<commit_message>
Adding a timetable handler
</commit_message>
<xml_diff>
--- a/AcousticsArrayTestLog.xlsx
+++ b/AcousticsArrayTestLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Mic 31 not working; ai0 not connected; Data located in "Testing 28JUL23" folder; Yohan tested</t>
+  </si>
+  <si>
+    <t>Mics 3 &amp; 31 not working; ai0 not connected; Data located in "Testing 2AUG2023" folder; 5 Bats Tested - 5th Bat was Rhino</t>
   </si>
 </sst>
 </file>
@@ -209,7 +212,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -606,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM6"/>
+  <dimension ref="A1:AM7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,13 +1348,141 @@
       </c>
       <c r="AM6" s="9"/>
     </row>
+    <row r="7" spans="1:39" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>45140</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM7" s="9"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G1:AL2 G5:AL5">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:AM2 G5:AM5">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:AL3">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:AM2 G5:AM5">
+  <conditionalFormatting sqref="G3:AM3">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -1329,12 +1490,12 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:AL3">
+  <conditionalFormatting sqref="G4:AL4">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:AM3">
+  <conditionalFormatting sqref="G4:AM4">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -1342,12 +1503,12 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:AL4">
+  <conditionalFormatting sqref="G7:AL7">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"NC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:AM4">
+  <conditionalFormatting sqref="G7:AM7">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>

</xml_diff>